<commit_message>
updated elec ces modeling
</commit_message>
<xml_diff>
--- a/InputData/elec/CRbQ/Cap Retirements before Quantization.xlsx
+++ b/InputData/elec/CRbQ/Cap Retirements before Quantization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\RMI\California\CA-eps\InputData\elec\CRbQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8C2056-8BC2-4B78-B940-6D5FF5735CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440788E6-5A72-4EC6-B91E-243BC4E7209F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9870" yWindow="255" windowWidth="16830" windowHeight="17175" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="14" r:id="rId1"/>
@@ -2450,8 +2450,8 @@
   </sheetPr>
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3351,8 +3351,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f>BCRbQ!C8</f>
-        <v>1300</v>
+        <v>1280</v>
       </c>
       <c r="E8">
         <f>BCRbQ!D8</f>

</xml_diff>